<commit_message>
try new model versions
</commit_message>
<xml_diff>
--- a/Analysis/model params.xlsx
+++ b/Analysis/model params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmgor\Dropbox\Taylor Chapter 3\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmgor\Dropbox\Taylor Chapter 3\Predict_Maturity\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE58FEC-D9EB-4EEF-8C89-B60C70EEE6F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D789DE-7D59-44BF-9CA6-73C8CF5D273C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A940222-3515-42B1-BE70-B71527DFFC76}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{4A940222-3515-42B1-BE70-B71527DFFC76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>habitat</t>
   </si>
@@ -98,9 +98,6 @@
     <t>body size relates to age at maturity</t>
   </si>
   <si>
-    <t>Frisk et al 2011</t>
-  </si>
-  <si>
     <t>life expectancy relates to age at maturity</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
   </si>
   <si>
     <t>interbirth interval relates to lifespan</t>
-  </si>
-  <si>
-    <t>life span relates to slope of maturity curve</t>
   </si>
   <si>
     <t>juvenile survivorship relates to age at maturity</t>
@@ -129,9 +123,6 @@
 Juvenile survivorship is related to age at maturity or body size or growth rate 13</t>
   </si>
   <si>
-    <t xml:space="preserve">body size of offspring relates to body size of parent </t>
-  </si>
-  <si>
     <t>metabolic rate affects growth rate</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
     <t>depth relates to body size, age at maturity, and longevity</t>
   </si>
   <si>
-    <t>Frisk et al 2011, Jennings et al 1998, Myers 1997</t>
-  </si>
-  <si>
     <t>Pauly et al 1998</t>
   </si>
   <si>
@@ -177,40 +165,16 @@
     <t>fecundity relates to body size</t>
   </si>
   <si>
-    <t>multiple refs</t>
-  </si>
-  <si>
     <t>size of offspring relates to body size of parent</t>
   </si>
   <si>
     <t>growth rate relates to slope of maturity curve because faster growth rate = narrower window of maturation</t>
   </si>
   <si>
-    <t>temp affects metabolic rate (16) &gt; metabolic rate affects growth rate (15) &gt; growth rate affects age at maturity (3)
-growth rate also affects slope of maturity curve (8)</t>
-  </si>
-  <si>
     <t>life expectancy relates to k</t>
   </si>
   <si>
-    <t>basically the same thing as a50 because ages are often back calculated from length</t>
-  </si>
-  <si>
     <t>general note</t>
-  </si>
-  <si>
-    <t>growth rate k relates to longevity/body size</t>
-  </si>
-  <si>
-    <t>Frisk 2011?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecundity relates body size (12) and body size in turn relates to age at maturity (1) 
-body size relates to life expectancy (5), life expectancy relates to growth rate (20) growth rate affects s (8)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">higher trophic level relates to larger body size (9) &gt; body size relates to age at maturity (1) 
-body size relates to life expectancy (5), life expectancy relates to growth rate (20) growth rate affects s (8)  </t>
   </si>
   <si>
     <t xml:space="preserve">size of offspring must relate to body size of parent (19) &gt; body size of parent relates to age at maturity (1) 
@@ -221,14 +185,6 @@
 body size relates to life expectancy (5), life expectancy relates to growth rate (20) growth rate affects s (8)  </t>
   </si>
   <si>
-    <t>animals with larger body size mature later (1). 
-body size relates to life expectancy (5), life expectancy relates to growth rate (20) growth rate affects s (8)  However, some discussion in Robbins 2006 about larger carcharhinid species growing quickly to avoid predation (the same as smaller species)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">longer interbirth interval indicates longer lifespan (10) which in turn means that interbirth interval is likely to affect a50
-life expectancy relates to growth rate (20) growth rate affects s (8)  </t>
-  </si>
-  <si>
     <t>habitat relates to body size, age at maturity, growth completion rate (k), and longevity (7)
 if habitat relates to body size, then relates to s as well (5, 20, 8)</t>
   </si>
@@ -263,9 +219,6 @@
     <t>take off s, doesn't seem to have an effect</t>
   </si>
   <si>
-    <t>remove from model, does same thing as lmax</t>
-  </si>
-  <si>
     <t>take offspring size off s, doesn't do anything</t>
   </si>
   <si>
@@ -273,6 +226,87 @@
   </si>
   <si>
     <t>change depth ave for max depth - has slightly larger effect</t>
+  </si>
+  <si>
+    <t>age at maturity decreases with increasing temperature</t>
+  </si>
+  <si>
+    <t>Myers &amp; Mertz 1997</t>
+  </si>
+  <si>
+    <t>Frisk et al 2001, Jennings et al 1998, Myers 1997</t>
+  </si>
+  <si>
+    <t>interbirth interval is part of fecundity (more frequent parturition=higher fecundity). Fecundity relates to body size (12) and body size relates to a50 (1)</t>
+  </si>
+  <si>
+    <t>litter size is part of fecundity (more frequent parturition=higher fecundity). Fecundity relates to body size (12) and body size relates to a50 (1)</t>
+  </si>
+  <si>
+    <t>remove from model, does same thing as lmax
+However, some discussion in Robbins 2006 about larger carcharhinid species growing quickly to avoid predation (the same as smaller species)</t>
+  </si>
+  <si>
+    <t>elasmobranchs prioritise survival over growth (from M/k ratio)</t>
+  </si>
+  <si>
+    <t>Frisk 2001</t>
+  </si>
+  <si>
+    <t>trophic level relates to body size (9), body size relates to a50 (1)
+trophic level relates to body size (9), body size relates to life expectancy (5), life expectancy relates to growth rate (20) growth rate affects s (8)</t>
+  </si>
+  <si>
+    <t>age at maturity decreases with increasing temperature (22)
+temperature relates to pop. growth rate (25) growth rate relates to S (3)</t>
+  </si>
+  <si>
+    <t>Holden 1974, Cortes 2000</t>
+  </si>
+  <si>
+    <t>Cortes 2000</t>
+  </si>
+  <si>
+    <t>negative relationship between litter size and offspring size once accounted for body size</t>
+  </si>
+  <si>
+    <r>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K negatively correlated with body size</t>
+    </r>
+  </si>
+  <si>
+    <t>Frisk 2001 (Cortes 2000 says only true for male sharks)</t>
+  </si>
+  <si>
+    <t>Frisk 2001, Cortes 2000</t>
+  </si>
+  <si>
+    <t>a50 positively correlated with lmat</t>
+  </si>
+  <si>
+    <t>a50 positively correlated with lmat (28)</t>
+  </si>
+  <si>
+    <t>individual growth rate increases with increasing temps</t>
   </si>
 </sst>
 </file>
@@ -282,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,8 +347,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,8 +380,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -386,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -406,7 +464,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -722,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A94D5AF-26EC-44F3-8E87-EFDC6EBBA2D4}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,7 +801,7 @@
     <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="88.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="43.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,7 +818,7 @@
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -764,7 +832,7 @@
         <v>18</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -774,11 +842,14 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -788,11 +859,14 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -802,22 +876,28 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -831,10 +911,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -842,234 +922,225 @@
         <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="15" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="16" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="C24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="C26">
         <v>7</v>
       </c>
-      <c r="D25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="C26">
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="C27">
         <v>8</v>
       </c>
-      <c r="D26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="C27">
-        <v>9</v>
-      </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
         <v>39</v>
@@ -1078,19 +1149,22 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="C28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="C29">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1099,10 +1173,10 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1111,100 +1185,150 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="C32" s="13">
+        <v>15</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="C32">
-        <v>14</v>
-      </c>
-      <c r="D32" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="2"/>
       <c r="C33">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="C34">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="C35">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-      <c r="C36">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>48</v>
+      <c r="C36" s="13">
+        <v>20</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="C37">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="C38">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
+      <c r="C39">
+        <v>25</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="C40" t="s">
-        <v>53</v>
+      <c r="C40">
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>74</v>
+      </c>
+      <c r="E40" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
+      <c r="C41">
+        <v>27</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>28</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="11"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>